<commit_message>
acrescentando coluna Seção e Equipe na consolidada
</commit_message>
<xml_diff>
--- a/start/TIN/TIN Telecom.xlsx
+++ b/start/TIN/TIN Telecom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://weg365.sharepoint.com/teams/BR-TI-TIN/Alocacao Recursos/TIN - Detalhamento Atividades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{D828C04F-A10E-4FAC-9D16-AC4898EEDA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2C32993-C3A4-4714-9AB8-10E38F8DDDAE}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:1_{D828C04F-A10E-4FAC-9D16-AC4898EEDA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C512A9E-0AFC-4FF2-88B2-966513FE43A8}"/>
   <bookViews>
-    <workbookView xWindow="-5970" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5970" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
@@ -1503,7 +1503,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1740,18 +1740,8 @@
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -7158,249 +7148,249 @@
       </c>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" s="84" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="82" t="s">
+    <row r="17" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="82" t="s">
+      <c r="C17" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D17" s="83">
+      <c r="D17" s="55">
         <v>2025</v>
       </c>
-      <c r="E17" s="84" t="s">
+      <c r="E17" t="s">
         <v>248</v>
       </c>
-      <c r="F17" s="85">
+      <c r="F17" s="19">
         <v>170</v>
       </c>
-      <c r="G17" s="86">
+      <c r="G17" s="49">
         <f t="shared" si="2"/>
         <v>170</v>
       </c>
-      <c r="H17" s="86">
+      <c r="H17" s="49">
         <v>30</v>
       </c>
-      <c r="I17" s="86">
+      <c r="I17" s="49">
         <v>120</v>
       </c>
-      <c r="J17" s="86">
+      <c r="J17" s="49">
         <v>20</v>
       </c>
-      <c r="K17" s="86">
-        <v>0</v>
-      </c>
-      <c r="L17" s="86">
-        <v>0</v>
-      </c>
-      <c r="M17" s="86">
-        <v>0</v>
-      </c>
-      <c r="N17" s="86">
-        <v>0</v>
-      </c>
-      <c r="O17" s="86">
-        <v>0</v>
-      </c>
-      <c r="P17" s="86">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="86">
-        <v>0</v>
-      </c>
-      <c r="R17" s="86">
-        <v>0</v>
-      </c>
-      <c r="S17" s="86">
-        <v>0</v>
-      </c>
-      <c r="T17" s="82"/>
-    </row>
-    <row r="18" spans="1:20" s="84" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="82" t="s">
+      <c r="K17" s="49">
+        <v>0</v>
+      </c>
+      <c r="L17" s="49">
+        <v>0</v>
+      </c>
+      <c r="M17" s="49">
+        <v>0</v>
+      </c>
+      <c r="N17" s="49">
+        <v>0</v>
+      </c>
+      <c r="O17" s="49">
+        <v>0</v>
+      </c>
+      <c r="P17" s="49">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="49">
+        <v>0</v>
+      </c>
+      <c r="R17" s="49">
+        <v>0</v>
+      </c>
+      <c r="S17" s="49">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="82" t="s">
+      <c r="B18" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="82" t="s">
+      <c r="C18" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D18" s="83">
+      <c r="D18" s="55">
         <v>2025</v>
       </c>
-      <c r="E18" s="84" t="s">
+      <c r="E18" t="s">
         <v>88</v>
       </c>
-      <c r="F18" s="85">
+      <c r="F18" s="19">
         <v>45</v>
       </c>
-      <c r="G18" s="86">
+      <c r="G18" s="49">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="H18" s="86">
+      <c r="H18" s="49">
         <v>10</v>
       </c>
-      <c r="I18" s="86">
+      <c r="I18" s="49">
         <v>30</v>
       </c>
-      <c r="J18" s="86">
+      <c r="J18" s="49">
         <v>5</v>
       </c>
-      <c r="K18" s="86">
-        <v>0</v>
-      </c>
-      <c r="L18" s="86">
-        <v>0</v>
-      </c>
-      <c r="M18" s="86">
-        <v>0</v>
-      </c>
-      <c r="N18" s="86">
-        <v>0</v>
-      </c>
-      <c r="O18" s="86">
-        <v>0</v>
-      </c>
-      <c r="P18" s="86">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="86">
-        <v>0</v>
-      </c>
-      <c r="R18" s="86">
-        <v>0</v>
-      </c>
-      <c r="S18" s="86">
-        <v>0</v>
-      </c>
-      <c r="T18" s="82"/>
-    </row>
-    <row r="19" spans="1:20" s="84" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="82" t="s">
+      <c r="K18" s="49">
+        <v>0</v>
+      </c>
+      <c r="L18" s="49">
+        <v>0</v>
+      </c>
+      <c r="M18" s="49">
+        <v>0</v>
+      </c>
+      <c r="N18" s="49">
+        <v>0</v>
+      </c>
+      <c r="O18" s="49">
+        <v>0</v>
+      </c>
+      <c r="P18" s="49">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="49">
+        <v>0</v>
+      </c>
+      <c r="R18" s="49">
+        <v>0</v>
+      </c>
+      <c r="S18" s="49">
+        <v>0</v>
+      </c>
+      <c r="T18" s="1"/>
+    </row>
+    <row r="19" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C19" s="82" t="s">
+      <c r="C19" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D19" s="83">
+      <c r="D19" s="55">
         <v>2025</v>
       </c>
-      <c r="E19" s="84" t="s">
+      <c r="E19" t="s">
         <v>248</v>
       </c>
-      <c r="F19" s="85">
+      <c r="F19" s="19">
         <v>230</v>
       </c>
-      <c r="G19" s="86">
+      <c r="G19" s="49">
         <f t="shared" si="2"/>
         <v>230</v>
       </c>
-      <c r="H19" s="86">
+      <c r="H19" s="49">
         <v>20</v>
       </c>
-      <c r="I19" s="86">
+      <c r="I19" s="49">
         <v>20</v>
       </c>
-      <c r="J19" s="86">
+      <c r="J19" s="49">
         <v>160</v>
       </c>
-      <c r="K19" s="86">
+      <c r="K19" s="49">
         <v>30</v>
       </c>
-      <c r="L19" s="86">
-        <v>0</v>
-      </c>
-      <c r="M19" s="86">
-        <v>0</v>
-      </c>
-      <c r="N19" s="86">
-        <v>0</v>
-      </c>
-      <c r="O19" s="86">
-        <v>0</v>
-      </c>
-      <c r="P19" s="86">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="86">
-        <v>0</v>
-      </c>
-      <c r="R19" s="86">
-        <v>0</v>
-      </c>
-      <c r="S19" s="86">
-        <v>0</v>
-      </c>
-      <c r="T19" s="82"/>
-    </row>
-    <row r="20" spans="1:20" s="84" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="82" t="s">
+      <c r="L19" s="49">
+        <v>0</v>
+      </c>
+      <c r="M19" s="49">
+        <v>0</v>
+      </c>
+      <c r="N19" s="49">
+        <v>0</v>
+      </c>
+      <c r="O19" s="49">
+        <v>0</v>
+      </c>
+      <c r="P19" s="49">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="49">
+        <v>0</v>
+      </c>
+      <c r="R19" s="49">
+        <v>0</v>
+      </c>
+      <c r="S19" s="49">
+        <v>0</v>
+      </c>
+      <c r="T19" s="1"/>
+    </row>
+    <row r="20" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C20" s="82" t="s">
+      <c r="C20" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D20" s="83">
+      <c r="D20" s="55">
         <v>2025</v>
       </c>
-      <c r="E20" s="84" t="s">
+      <c r="E20" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="85">
+      <c r="F20" s="19">
         <v>70</v>
       </c>
-      <c r="G20" s="86">
+      <c r="G20" s="49">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="H20" s="86">
+      <c r="H20" s="49">
         <v>10</v>
       </c>
-      <c r="I20" s="86">
+      <c r="I20" s="49">
         <v>10</v>
       </c>
-      <c r="J20" s="86">
+      <c r="J20" s="49">
         <v>40</v>
       </c>
-      <c r="K20" s="86">
+      <c r="K20" s="49">
         <v>10</v>
       </c>
-      <c r="L20" s="86">
-        <v>0</v>
-      </c>
-      <c r="M20" s="86">
-        <v>0</v>
-      </c>
-      <c r="N20" s="86">
-        <v>0</v>
-      </c>
-      <c r="O20" s="86">
-        <v>0</v>
-      </c>
-      <c r="P20" s="86">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="86">
-        <v>0</v>
-      </c>
-      <c r="R20" s="86">
-        <v>0</v>
-      </c>
-      <c r="S20" s="86">
-        <v>0</v>
-      </c>
-      <c r="T20" s="82"/>
+      <c r="L20" s="49">
+        <v>0</v>
+      </c>
+      <c r="M20" s="49">
+        <v>0</v>
+      </c>
+      <c r="N20" s="49">
+        <v>0</v>
+      </c>
+      <c r="O20" s="49">
+        <v>0</v>
+      </c>
+      <c r="P20" s="49">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="49">
+        <v>0</v>
+      </c>
+      <c r="R20" s="49">
+        <v>0</v>
+      </c>
+      <c r="S20" s="49">
+        <v>0</v>
+      </c>
+      <c r="T20" s="1"/>
     </row>
     <row r="21" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -11055,9 +11045,9 @@
   <sheetPr codeName="Planilha4"/>
   <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11069,8 +11059,7 @@
     <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="10.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="1" customWidth="1"/>
+    <col min="8" max="11" width="10.42578125" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="27" width="11.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11166,7 +11155,7 @@
       </c>
       <c r="G2" s="19">
         <f>SUM(Tabela1456[[#This Row],[ago/24]:[dez/25]])</f>
-        <v>1843</v>
+        <v>1831</v>
       </c>
       <c r="H2" s="23">
         <f>H3-H4</f>
@@ -11186,19 +11175,19 @@
       </c>
       <c r="L2" s="59">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="M2" s="59">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N2" s="59">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="O2" s="59">
         <f t="shared" si="0"/>
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P2" s="59">
         <f t="shared" ref="P2:AA2" si="1">P3-P4</f>
@@ -11331,7 +11320,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="11">
         <f>SUM(Tabela1456[[#This Row],[ago/24]:[dez/25]])</f>
-        <v>881</v>
+        <v>893</v>
       </c>
       <c r="H4" s="24">
         <f>SUM(H5:H31)</f>
@@ -11351,19 +11340,19 @@
       </c>
       <c r="L4" s="60">
         <f t="shared" si="2"/>
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="M4" s="60">
         <f t="shared" si="2"/>
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="N4" s="60">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="O4" s="60">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P4" s="60">
         <f t="shared" si="2"/>
@@ -11416,7 +11405,7 @@
       <c r="AB4" s="4"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="82" t="s">
         <v>144</v>
       </c>
       <c r="B5" s="17"/>
@@ -11430,7 +11419,7 @@
       </c>
       <c r="G5" s="19">
         <f>SUM(Tabela1456[[#This Row],[ago/24]:[dez/25]])</f>
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="H5" s="24">
         <v>27</v>
@@ -11445,7 +11434,7 @@
         <v>32</v>
       </c>
       <c r="L5" s="53">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M5" s="53">
         <v>31</v>
@@ -11814,7 +11803,7 @@
       </c>
       <c r="G10" s="19">
         <f>SUM(Tabela1456[[#This Row],[ago/24]:[dez/25]])</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H10" s="25">
         <v>24</v>
@@ -11829,7 +11818,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M10" s="16">
         <v>0</v>
@@ -11896,7 +11885,7 @@
       </c>
       <c r="G11" s="19">
         <f>SUM(Tabela1456[[#This Row],[ago/24]:[dez/25]])</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H11" s="25">
         <v>8</v>
@@ -11911,7 +11900,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M11" s="16">
         <v>0</v>
@@ -12113,7 +12102,7 @@
       <c r="AB13" s="58"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="66" t="s">
         <v>153</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -12133,7 +12122,7 @@
       </c>
       <c r="G14" s="19">
         <f>SUM(Tabela1456[[#This Row],[ago/24]:[dez/25]])</f>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="5">
@@ -12146,7 +12135,7 @@
         <v>13</v>
       </c>
       <c r="L14" s="16">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="M14" s="16">
         <v>0</v>
@@ -12513,7 +12502,7 @@
       </c>
       <c r="G19" s="19">
         <f>SUM(Tabela1456[[#This Row],[ago/24]:[dez/25]])</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -12524,7 +12513,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M19" s="16">
         <v>0</v>
@@ -12591,7 +12580,7 @@
       </c>
       <c r="G20" s="19">
         <f>SUM(Tabela1456[[#This Row],[ago/24]:[dez/25]])</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -12602,7 +12591,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M20" s="16">
         <v>0</v>
@@ -12815,7 +12804,7 @@
       </c>
       <c r="G23" s="19">
         <f>SUM(Tabela1456[[#This Row],[ago/24]:[dez/25]])</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H23" s="25">
         <v>8</v>
@@ -12830,7 +12819,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M23" s="16">
         <v>0</v>
@@ -12912,13 +12901,13 @@
         <v>0</v>
       </c>
       <c r="L24" s="16">
+        <v>0</v>
+      </c>
+      <c r="M24" s="16">
         <v>8</v>
       </c>
-      <c r="M24" s="16">
+      <c r="N24" s="16">
         <v>4</v>
-      </c>
-      <c r="N24" s="16">
-        <v>0</v>
       </c>
       <c r="O24" s="16">
         <v>0</v>
@@ -12979,7 +12968,7 @@
       </c>
       <c r="G25" s="19">
         <f>SUM(Tabela1456[[#This Row],[ago/24]:[dez/25]])</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H25" s="25">
         <v>0</v>
@@ -12994,16 +12983,16 @@
         <v>0</v>
       </c>
       <c r="L25" s="16">
+        <v>0</v>
+      </c>
+      <c r="M25" s="16">
+        <v>0</v>
+      </c>
+      <c r="N25" s="16">
+        <v>8</v>
+      </c>
+      <c r="O25" s="16">
         <v>2</v>
-      </c>
-      <c r="M25" s="16">
-        <v>0</v>
-      </c>
-      <c r="N25" s="16">
-        <v>0</v>
-      </c>
-      <c r="O25" s="16">
-        <v>0</v>
       </c>
       <c r="P25" s="16">
         <v>0</v>
@@ -13504,7 +13493,7 @@
       <c r="AB31" s="58"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="66" t="s">
         <v>69</v>
       </c>
       <c r="C32" s="33" t="s">
@@ -13521,7 +13510,7 @@
       </c>
       <c r="G32" s="19">
         <f>SUM(Tabela1456[[#This Row],[ago/24]:[dez/25]])</f>
-        <v>194</v>
+        <v>228</v>
       </c>
       <c r="H32" s="26"/>
       <c r="I32" s="18">
@@ -13534,7 +13523,7 @@
         <v>113</v>
       </c>
       <c r="L32" s="16">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="M32" s="16">
         <v>1</v>
@@ -13602,7 +13591,7 @@
       </c>
       <c r="G33" s="19">
         <f>SUM(Tabela1456[[#This Row],[ago/24]:[dez/25]])</f>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="5"/>
@@ -13611,7 +13600,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M33" s="16">
         <v>4</v>
@@ -13679,7 +13668,7 @@
       </c>
       <c r="G34" s="19">
         <f>SUM(Tabela1456[[#This Row],[ago/24]:[dez/25]])</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="5"/>
@@ -13690,7 +13679,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="16">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M34" s="16">
         <v>0</v>
@@ -14184,7 +14173,7 @@
       <formula>IF(#REF!=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22:A25 A28 H31:H34 J31:O31 J46:O46 N32:O32 H35:L35 H6:AA7 V13:AA15 V18:AA20 V22:AA25 V28:AA30 H22:O26 H9:AA12 H8:AB8 H28:O28 V32:AA36 H36:H46">
+  <conditionalFormatting sqref="A22:A25 A28 H31:H34 J31:O31 J46:O46 N32:O32 H35:L35 H6:AA7 V13:AA15 V18:AA20 V22:AA25 V28:AA30 H9:AA12 H8:AB8 H28:O28 V32:AA36 H36:H46 H22:O26">
     <cfRule type="expression" dxfId="529" priority="121">
       <formula>IF($A6="Esforço total atribuído",1)</formula>
     </cfRule>
@@ -15262,10 +15251,10 @@
   <sheetPr codeName="Planilha6"/>
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B44" sqref="B44"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17137,7 +17126,7 @@
       <c r="AB25" s="1"/>
     </row>
     <row r="26" spans="1:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="82" t="s">
+      <c r="A26" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -26132,6 +26121,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010055299C8A5E56DF42BB3A496FAB31A3CA" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="f48546ee30a9c08b8c56cc99cae99613">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="886f8626-7949-4fe5-8403-a629ca357b95" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4da67acbd85d4947d1135fd4f9dd5422" ns2:_="">
     <xsd:import namespace="886f8626-7949-4fe5-8403-a629ca357b95"/>
@@ -26275,18 +26275,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{076963EF-7E18-4286-B416-ADA05C6F6E23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="886f8626-7949-4fe5-8403-a629ca357b95"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E1C848C-A0C9-41E4-8BB1-646104CE90D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{790518B7-6307-4320-A86D-39C8BAC5E03D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26304,30 +26317,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E1C848C-A0C9-41E4-8BB1-646104CE90D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{076963EF-7E18-4286-B416-ADA05C6F6E23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="886f8626-7949-4fe5-8403-a629ca357b95"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{886666a6-a8d2-4604-a002-95b622cb7e18}" enabled="0" method="" siteId="{886666a6-a8d2-4604-a002-95b622cb7e18}" removed="1"/>

</xml_diff>